<commit_message>
fix Dob loader issue + Address Teacher IssueIssue
</commit_message>
<xml_diff>
--- a/web/backend/Python-services/src/data/xlsx/sample/FAMS_10.xlsx
+++ b/web/backend/Python-services/src/data/xlsx/sample/FAMS_10.xlsx
@@ -880,7 +880,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -890,13 +890,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -943,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -954,10 +948,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -965,6 +959,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,7 +1272,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -1289,7 +1286,7 @@
     <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>90</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>97</v>
       </c>
@@ -1406,7 +1403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>101</v>
       </c>
@@ -1441,7 +1438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>106</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>111</v>
       </c>
@@ -1517,7 +1514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>117</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>122</v>
       </c>
@@ -1587,7 +1584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>126</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>130</v>
       </c>
@@ -1669,7 +1666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>133</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>137</v>
       </c>
@@ -1745,7 +1742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>141</v>
       </c>
@@ -1786,7 +1783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>146</v>
       </c>
@@ -1821,7 +1818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>150</v>
       </c>
@@ -1856,7 +1853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>153</v>
       </c>
@@ -1891,7 +1888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
         <v>156</v>
       </c>
@@ -1926,7 +1923,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>159</v>
       </c>
@@ -1961,7 +1958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
         <v>162</v>
       </c>
@@ -1996,7 +1993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>158</v>
       </c>
@@ -2037,7 +2034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -2072,7 +2069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>172</v>
       </c>
@@ -2107,7 +2104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>122</v>
       </c>
@@ -2148,7 +2145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
         <v>178</v>
       </c>
@@ -2183,7 +2180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
         <v>182</v>
       </c>
@@ -2224,7 +2221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>187</v>
       </c>
@@ -2259,7 +2256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3" t="s">
         <v>59</v>
       </c>
@@ -2300,7 +2297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3" t="s">
         <v>133</v>
       </c>
@@ -2335,7 +2332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
@@ -2405,7 +2402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3" t="s">
         <v>204</v>
       </c>
@@ -2440,7 +2437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3" t="s">
         <v>193</v>
       </c>
@@ -2475,7 +2472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3" t="s">
         <v>208</v>
       </c>
@@ -2510,7 +2507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="3" t="s">
         <v>66</v>
       </c>
@@ -3593,7 +3590,7 @@
     <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>

</xml_diff>

<commit_message>
update format data, attendance API
</commit_message>
<xml_diff>
--- a/web/backend/Python-services/src/data/xlsx/sample/FAMS_10.xlsx
+++ b/web/backend/Python-services/src/data/xlsx/sample/FAMS_10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384C3B1F-52FD-44C9-B222-BD1DF89CD412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C9C66C-8585-4DDC-96AD-417A64FB1428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1619" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="715">
   <si>
     <t>Họ và Tên</t>
   </si>
@@ -1820,790 +1820,10 @@
     <t>phamthanhkhanh774@gmail.com</t>
   </si>
   <si>
-    <t>Nguyễn Ngọc Hùng</t>
-  </si>
-  <si>
-    <t>20/07/2009</t>
-  </si>
-  <si>
-    <t>0986555918</t>
-  </si>
-  <si>
-    <t>Phạm Văn Trang</t>
-  </si>
-  <si>
-    <t>0930777205</t>
-  </si>
-  <si>
-    <t>phamvantrang193@gmail.com</t>
-  </si>
-  <si>
-    <t>Võ Thanh Lan</t>
-  </si>
-  <si>
-    <t>0985448038</t>
-  </si>
-  <si>
-    <t>vothanhlan717@gmail.com</t>
-  </si>
-  <si>
-    <t>Đặng Xuân Trang</t>
-  </si>
-  <si>
-    <t>02/10/2009</t>
-  </si>
-  <si>
-    <t>0940137455</t>
-  </si>
-  <si>
-    <t>Đặng Thanh An</t>
-  </si>
-  <si>
-    <t>0953772398</t>
-  </si>
-  <si>
-    <t>đangthanhan208@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Ngọc Quân</t>
-  </si>
-  <si>
-    <t>18/06/2009</t>
-  </si>
-  <si>
-    <t>0910491559</t>
-  </si>
-  <si>
-    <t>Đỗ Thị Chi</t>
-  </si>
-  <si>
-    <t>0982499264</t>
-  </si>
-  <si>
-    <t>đothichi332@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Thanh Tú</t>
-  </si>
-  <si>
-    <t>25/10/2009</t>
-  </si>
-  <si>
-    <t>0926004341</t>
-  </si>
-  <si>
-    <t>Võ Xuân Dũng</t>
-  </si>
-  <si>
-    <t>0904947086</t>
-  </si>
-  <si>
-    <t>voxuandung215@gmail.com</t>
-  </si>
-  <si>
-    <t>0978233545</t>
-  </si>
-  <si>
-    <t>nguyenngochung671@gmail.com</t>
-  </si>
-  <si>
-    <t>Bùi Thanh Hà</t>
-  </si>
-  <si>
-    <t>05/03/2009</t>
-  </si>
-  <si>
-    <t>0959135172</t>
-  </si>
-  <si>
-    <t>0919947016</t>
-  </si>
-  <si>
-    <t>nguyenminhkhanh798@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyễn Ngọc Lan</t>
-  </si>
-  <si>
-    <t>0924968534</t>
-  </si>
-  <si>
-    <t>Võ Minh Hà</t>
-  </si>
-  <si>
-    <t>0937915051</t>
-  </si>
-  <si>
-    <t>vominhha309@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Xuân Hà</t>
-  </si>
-  <si>
-    <t>22/05/2009</t>
-  </si>
-  <si>
-    <t>0959174657</t>
-  </si>
-  <si>
-    <t>Đỗ Xuân Hà</t>
-  </si>
-  <si>
-    <t>0983304544</t>
-  </si>
-  <si>
-    <t>đoxuanha443@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Xuân Mai</t>
-  </si>
-  <si>
-    <t>0934030501</t>
-  </si>
-  <si>
-    <t>đoxuanmai768@gmail.com</t>
-  </si>
-  <si>
-    <t>Hoàng Minh Phúc</t>
-  </si>
-  <si>
-    <t>0992992517</t>
-  </si>
-  <si>
-    <t>Lê Xuân Hà</t>
-  </si>
-  <si>
-    <t>0949302923</t>
-  </si>
-  <si>
-    <t>lexuanha347@gmail.com</t>
-  </si>
-  <si>
-    <t>Bùi Xuân Dũng</t>
-  </si>
-  <si>
-    <t>0985389196</t>
-  </si>
-  <si>
-    <t>Võ Ngọc Tú</t>
-  </si>
-  <si>
-    <t>0924438849</t>
-  </si>
-  <si>
-    <t>vongoctu232@gmail.com</t>
-  </si>
-  <si>
-    <t>Bùi Xuân Hùng</t>
-  </si>
-  <si>
-    <t>0952757987</t>
-  </si>
-  <si>
-    <t>buixuanhung641@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Mai</t>
-  </si>
-  <si>
-    <t>0932340452</t>
-  </si>
-  <si>
-    <t>Đỗ Minh Chi</t>
-  </si>
-  <si>
-    <t>0994443422</t>
-  </si>
-  <si>
-    <t>đominhchi656@gmail.com</t>
-  </si>
-  <si>
-    <t>Trần Thị Tú</t>
-  </si>
-  <si>
-    <t>12/11/2009</t>
-  </si>
-  <si>
-    <t>0960622038</t>
-  </si>
-  <si>
-    <t>0955599864</t>
-  </si>
-  <si>
-    <t>tranthanhquan183@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Văn Khánh</t>
-  </si>
-  <si>
-    <t>0961288203</t>
-  </si>
-  <si>
-    <t>levankhanh867@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyễn Hữu Quân</t>
-  </si>
-  <si>
-    <t>0949953733</t>
-  </si>
-  <si>
-    <t>Trần Thanh Mai</t>
-  </si>
-  <si>
-    <t>0920441171</t>
-  </si>
-  <si>
-    <t>tranthanhmai831@gmail.com</t>
-  </si>
-  <si>
-    <t>17/08/2009</t>
-  </si>
-  <si>
-    <t>0993251207</t>
-  </si>
-  <si>
-    <t>Võ Thanh Hà</t>
-  </si>
-  <si>
-    <t>0963658608</t>
-  </si>
-  <si>
-    <t>vothanhha293@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Hữu Chi</t>
-  </si>
-  <si>
-    <t>10/07/2009</t>
-  </si>
-  <si>
-    <t>0923994802</t>
-  </si>
-  <si>
-    <t>Lê Thanh Quân</t>
-  </si>
-  <si>
-    <t>0946587291</t>
-  </si>
-  <si>
-    <t>lethanhquan773@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Thị Phúc</t>
-  </si>
-  <si>
-    <t>0964562978</t>
-  </si>
-  <si>
-    <t>đothiphuc150@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Ngọc Hà</t>
-  </si>
-  <si>
-    <t>28/11/2009</t>
-  </si>
-  <si>
-    <t>0994347404</t>
-  </si>
-  <si>
-    <t>Phạm Hữu Hà</t>
-  </si>
-  <si>
-    <t>0956055253</t>
-  </si>
-  <si>
-    <t>phamhuuha656@gmail.com</t>
-  </si>
-  <si>
-    <t>Võ Minh Bình</t>
-  </si>
-  <si>
-    <t>0911480093</t>
-  </si>
-  <si>
-    <t>vominhbinh431@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Ngọc Mai</t>
-  </si>
-  <si>
-    <t>19/09/2009</t>
-  </si>
-  <si>
-    <t>0910252979</t>
-  </si>
-  <si>
-    <t>Lê Minh Hà</t>
-  </si>
-  <si>
-    <t>0911752735</t>
-  </si>
-  <si>
-    <t>leminhha523@gmail.com</t>
-  </si>
-  <si>
-    <t>Bùi Minh Dũng</t>
-  </si>
-  <si>
-    <t>08/04/2009</t>
-  </si>
-  <si>
-    <t>0949309142</t>
-  </si>
-  <si>
-    <t>Hoàng Văn Trang</t>
-  </si>
-  <si>
-    <t>0907524437</t>
-  </si>
-  <si>
-    <t>hoangvantrang934@gmail.com</t>
-  </si>
-  <si>
     <t>Nguyễn Thị Nam</t>
   </si>
   <si>
-    <t>24/10/2009</t>
-  </si>
-  <si>
-    <t>0912661510</t>
-  </si>
-  <si>
-    <t>Hoàng Văn Tú</t>
-  </si>
-  <si>
-    <t>0939648144</t>
-  </si>
-  <si>
-    <t>hoangvantu945@gmail.com</t>
-  </si>
-  <si>
-    <t>Võ Ngọc Mai</t>
-  </si>
-  <si>
-    <t>05/06/2009</t>
-  </si>
-  <si>
-    <t>0901033922</t>
-  </si>
-  <si>
-    <t>Phạm Thanh Nam</t>
-  </si>
-  <si>
-    <t>0980463503</t>
-  </si>
-  <si>
-    <t>phamthanhnam204@gmail.com</t>
-  </si>
-  <si>
-    <t>Đặng Ngọc Quân</t>
-  </si>
-  <si>
-    <t>0921602241</t>
-  </si>
-  <si>
-    <t>đangngocquan647@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Thanh Dũng</t>
-  </si>
-  <si>
-    <t>27/09/2009</t>
-  </si>
-  <si>
-    <t>0947858272</t>
-  </si>
-  <si>
-    <t>Bùi Văn Phúc</t>
-  </si>
-  <si>
-    <t>0931262356</t>
-  </si>
-  <si>
-    <t>buivanphuc453@gmail.com</t>
-  </si>
-  <si>
-    <t>Đặng Minh Hà</t>
-  </si>
-  <si>
-    <t>12/08/2009</t>
-  </si>
-  <si>
-    <t>0960731728</t>
-  </si>
-  <si>
-    <t>0902875658</t>
-  </si>
-  <si>
-    <t>huynhxuannam470@gmail.com</t>
-  </si>
-  <si>
-    <t>Hoàng Văn Hà</t>
-  </si>
-  <si>
-    <t>07/10/2009</t>
-  </si>
-  <si>
-    <t>0941963842</t>
-  </si>
-  <si>
-    <t>Huỳnh Văn Trang</t>
-  </si>
-  <si>
-    <t>0919405350</t>
-  </si>
-  <si>
-    <t>huynhvantrang493@gmail.com</t>
-  </si>
-  <si>
-    <t>06/10/2009</t>
-  </si>
-  <si>
-    <t>0934091589</t>
-  </si>
-  <si>
-    <t>Đỗ Thị Lan</t>
-  </si>
-  <si>
-    <t>0962298677</t>
-  </si>
-  <si>
-    <t>đothilan283@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Thanh Hà</t>
-  </si>
-  <si>
-    <t>03/01/2009</t>
-  </si>
-  <si>
-    <t>0927572473</t>
-  </si>
-  <si>
-    <t>Lê Hữu Nam</t>
-  </si>
-  <si>
-    <t>0945573299</t>
-  </si>
-  <si>
-    <t>lehuunam325@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Xuân Mai</t>
-  </si>
-  <si>
-    <t>07/07/2009</t>
-  </si>
-  <si>
-    <t>0975570756</t>
-  </si>
-  <si>
-    <t>Trần Văn An</t>
-  </si>
-  <si>
-    <t>0991543649</t>
-  </si>
-  <si>
-    <t>tranvanan344@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Thanh Phúc</t>
-  </si>
-  <si>
-    <t>16/05/2009</t>
-  </si>
-  <si>
-    <t>0986102570</t>
-  </si>
-  <si>
-    <t>Huỳnh Thị Mai</t>
-  </si>
-  <si>
-    <t>0949383950</t>
-  </si>
-  <si>
-    <t>huynhthimai562@gmail.com</t>
-  </si>
-  <si>
-    <t>Đặng Minh Chi</t>
-  </si>
-  <si>
-    <t>0981563786</t>
-  </si>
-  <si>
-    <t>đangminhchi818@gmail.com</t>
-  </si>
-  <si>
-    <t>Trần Thị Như</t>
-  </si>
-  <si>
-    <t>21/12/2009</t>
-  </si>
-  <si>
-    <t>0924790210</t>
-  </si>
-  <si>
-    <t>Phạm Minh Dũng</t>
-  </si>
-  <si>
-    <t>0984047062</t>
-  </si>
-  <si>
-    <t>phamminhdung309@gmail.com</t>
-  </si>
-  <si>
     <t>Đặng Văn Như</t>
-  </si>
-  <si>
-    <t>07/02/2009</t>
-  </si>
-  <si>
-    <t>0976088602</t>
-  </si>
-  <si>
-    <t>Hoàng Văn Dũng</t>
-  </si>
-  <si>
-    <t>0943970094</t>
-  </si>
-  <si>
-    <t>hoangvandung779@gmail.com</t>
-  </si>
-  <si>
-    <t>25/04/2009</t>
-  </si>
-  <si>
-    <t>0991831670</t>
-  </si>
-  <si>
-    <t>Hoàng Minh Quân</t>
-  </si>
-  <si>
-    <t>0922175758</t>
-  </si>
-  <si>
-    <t>hoangminhquan995@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Thị Tú</t>
-  </si>
-  <si>
-    <t>04/01/2009</t>
-  </si>
-  <si>
-    <t>0909547331</t>
-  </si>
-  <si>
-    <t>Hoàng Thanh Trang</t>
-  </si>
-  <si>
-    <t>0936608745</t>
-  </si>
-  <si>
-    <t>hoangthanhtrang500@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Văn Hà</t>
-  </si>
-  <si>
-    <t>0983933743</t>
-  </si>
-  <si>
-    <t>đovanha137@gmail.com</t>
-  </si>
-  <si>
-    <t>04/06/2009</t>
-  </si>
-  <si>
-    <t>0918078810</t>
-  </si>
-  <si>
-    <t>Hoàng Ngọc Dũng</t>
-  </si>
-  <si>
-    <t>0983736773</t>
-  </si>
-  <si>
-    <t>hoangngocdung998@gmail.com</t>
-  </si>
-  <si>
-    <t>0903368961</t>
-  </si>
-  <si>
-    <t>đangthanhbinh801@gmail.com</t>
-  </si>
-  <si>
-    <t>Trần Thanh Hà</t>
-  </si>
-  <si>
-    <t>08/02/2009</t>
-  </si>
-  <si>
-    <t>0965543940</t>
-  </si>
-  <si>
-    <t>Nguyễn Xuân Lan</t>
-  </si>
-  <si>
-    <t>0956004155</t>
-  </si>
-  <si>
-    <t>nguyenxuanlan203@gmail.com</t>
-  </si>
-  <si>
-    <t>Võ Xuân Trang</t>
-  </si>
-  <si>
-    <t>0900585345</t>
-  </si>
-  <si>
-    <t>voxuantrang920@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Xuân Tú</t>
-  </si>
-  <si>
-    <t>16/11/2009</t>
-  </si>
-  <si>
-    <t>0935960932</t>
-  </si>
-  <si>
-    <t>Lê Xuân Khánh</t>
-  </si>
-  <si>
-    <t>0998130940</t>
-  </si>
-  <si>
-    <t>lexuankhanh368@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Thị Dũng</t>
-  </si>
-  <si>
-    <t>16/03/2009</t>
-  </si>
-  <si>
-    <t>0975146570</t>
-  </si>
-  <si>
-    <t>Trần Xuân Lan</t>
-  </si>
-  <si>
-    <t>0973842300</t>
-  </si>
-  <si>
-    <t>tranxuanlan468@gmail.com</t>
-  </si>
-  <si>
-    <t>Đỗ Văn Trang</t>
-  </si>
-  <si>
-    <t>0946515210</t>
-  </si>
-  <si>
-    <t>đovantrang755@gmail.com</t>
-  </si>
-  <si>
-    <t>Đặng Ngọc Dũng</t>
-  </si>
-  <si>
-    <t>15/09/2009</t>
-  </si>
-  <si>
-    <t>0990441016</t>
-  </si>
-  <si>
-    <t>Trần Minh Phúc</t>
-  </si>
-  <si>
-    <t>0980246780</t>
-  </si>
-  <si>
-    <t>tranminhphuc352@gmail.com</t>
-  </si>
-  <si>
-    <t>Trần Minh Nam</t>
-  </si>
-  <si>
-    <t>13/02/2009</t>
-  </si>
-  <si>
-    <t>0949333990</t>
-  </si>
-  <si>
-    <t>Lê Thị Hùng</t>
-  </si>
-  <si>
-    <t>0937492776</t>
-  </si>
-  <si>
-    <t>lethihung165@gmail.com</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Mai</t>
-  </si>
-  <si>
-    <t>24/03/2009</t>
-  </si>
-  <si>
-    <t>0993799258</t>
-  </si>
-  <si>
-    <t>0952978564</t>
-  </si>
-  <si>
-    <t>đongocan722@gmail.com</t>
-  </si>
-  <si>
-    <t>Phạm Thanh Bình</t>
-  </si>
-  <si>
-    <t>0967253698</t>
-  </si>
-  <si>
-    <t>Nguyễn Hữu Trang</t>
-  </si>
-  <si>
-    <t>0938979866</t>
-  </si>
-  <si>
-    <t>nguyenhuutrang289@gmail.com</t>
-  </si>
-  <si>
-    <t>0999663451</t>
-  </si>
-  <si>
-    <t>hoangthian346@gmail.com</t>
-  </si>
-  <si>
-    <t>Huỳnh Thị Hùng</t>
-  </si>
-  <si>
-    <t>0962479159</t>
-  </si>
-  <si>
-    <t>Bùi Xuân Mai</t>
-  </si>
-  <si>
-    <t>0976539551</t>
-  </si>
-  <si>
-    <t>buixuanmai508@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Ngọc Bình</t>
-  </si>
-  <si>
-    <t>0906533411</t>
-  </si>
-  <si>
-    <t>0990011758</t>
-  </si>
-  <si>
-    <t>đovanha252@gmail.com</t>
   </si>
   <si>
     <t>Email</t>
@@ -3017,7 +2237,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3322,10 +2542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P121"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="P121" sqref="A82:P121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3382,7 +2602,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>974</v>
+        <v>714</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -6438,1496 +5658,6 @@
       </c>
       <c r="O81" t="s">
         <v>598</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>599</v>
-      </c>
-      <c r="B82" t="s">
-        <v>600</v>
-      </c>
-      <c r="C82" t="s">
-        <v>23</v>
-      </c>
-      <c r="D82" t="s">
-        <v>56</v>
-      </c>
-      <c r="E82" t="s">
-        <v>601</v>
-      </c>
-      <c r="F82" t="s">
-        <v>602</v>
-      </c>
-      <c r="G82" t="s">
-        <v>37</v>
-      </c>
-      <c r="H82" t="s">
-        <v>603</v>
-      </c>
-      <c r="I82" t="s">
-        <v>23</v>
-      </c>
-      <c r="J82" t="s">
-        <v>604</v>
-      </c>
-      <c r="K82" t="s">
-        <v>605</v>
-      </c>
-      <c r="L82" t="s">
-        <v>83</v>
-      </c>
-      <c r="M82" t="s">
-        <v>606</v>
-      </c>
-      <c r="N82" t="s">
-        <v>17</v>
-      </c>
-      <c r="O82" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>608</v>
-      </c>
-      <c r="B83" t="s">
-        <v>609</v>
-      </c>
-      <c r="C83" t="s">
-        <v>23</v>
-      </c>
-      <c r="D83" t="s">
-        <v>49</v>
-      </c>
-      <c r="E83" t="s">
-        <v>610</v>
-      </c>
-      <c r="F83" t="s">
-        <v>611</v>
-      </c>
-      <c r="G83" t="s">
-        <v>83</v>
-      </c>
-      <c r="H83" t="s">
-        <v>612</v>
-      </c>
-      <c r="I83" t="s">
-        <v>17</v>
-      </c>
-      <c r="J83" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>614</v>
-      </c>
-      <c r="B84" t="s">
-        <v>615</v>
-      </c>
-      <c r="C84" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" t="s">
-        <v>56</v>
-      </c>
-      <c r="E84" t="s">
-        <v>616</v>
-      </c>
-      <c r="F84" t="s">
-        <v>617</v>
-      </c>
-      <c r="G84" t="s">
-        <v>21</v>
-      </c>
-      <c r="H84" t="s">
-        <v>618</v>
-      </c>
-      <c r="I84" t="s">
-        <v>17</v>
-      </c>
-      <c r="J84" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>620</v>
-      </c>
-      <c r="B85" t="s">
-        <v>621</v>
-      </c>
-      <c r="C85" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" t="s">
-        <v>49</v>
-      </c>
-      <c r="E85" t="s">
-        <v>622</v>
-      </c>
-      <c r="F85" t="s">
-        <v>623</v>
-      </c>
-      <c r="G85" t="s">
-        <v>21</v>
-      </c>
-      <c r="H85" t="s">
-        <v>624</v>
-      </c>
-      <c r="I85" t="s">
-        <v>17</v>
-      </c>
-      <c r="J85" t="s">
-        <v>625</v>
-      </c>
-      <c r="K85" t="s">
-        <v>599</v>
-      </c>
-      <c r="L85" t="s">
-        <v>30</v>
-      </c>
-      <c r="M85" t="s">
-        <v>626</v>
-      </c>
-      <c r="N85" t="s">
-        <v>23</v>
-      </c>
-      <c r="O85" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>628</v>
-      </c>
-      <c r="B86" t="s">
-        <v>629</v>
-      </c>
-      <c r="C86" t="s">
-        <v>17</v>
-      </c>
-      <c r="D86" t="s">
-        <v>91</v>
-      </c>
-      <c r="E86" t="s">
-        <v>630</v>
-      </c>
-      <c r="F86" t="s">
-        <v>51</v>
-      </c>
-      <c r="G86" t="s">
-        <v>76</v>
-      </c>
-      <c r="H86" t="s">
-        <v>631</v>
-      </c>
-      <c r="I86" t="s">
-        <v>17</v>
-      </c>
-      <c r="J86" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>633</v>
-      </c>
-      <c r="B87" t="s">
-        <v>213</v>
-      </c>
-      <c r="C87" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" t="s">
-        <v>42</v>
-      </c>
-      <c r="E87" t="s">
-        <v>634</v>
-      </c>
-      <c r="F87" t="s">
-        <v>635</v>
-      </c>
-      <c r="G87" t="s">
-        <v>30</v>
-      </c>
-      <c r="H87" t="s">
-        <v>636</v>
-      </c>
-      <c r="I87" t="s">
-        <v>17</v>
-      </c>
-      <c r="J87" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>638</v>
-      </c>
-      <c r="B88" t="s">
-        <v>639</v>
-      </c>
-      <c r="C88" t="s">
-        <v>17</v>
-      </c>
-      <c r="D88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E88" t="s">
-        <v>640</v>
-      </c>
-      <c r="F88" t="s">
-        <v>641</v>
-      </c>
-      <c r="G88" t="s">
-        <v>94</v>
-      </c>
-      <c r="H88" t="s">
-        <v>642</v>
-      </c>
-      <c r="I88" t="s">
-        <v>17</v>
-      </c>
-      <c r="J88" t="s">
-        <v>643</v>
-      </c>
-      <c r="K88" t="s">
-        <v>644</v>
-      </c>
-      <c r="L88" t="s">
-        <v>83</v>
-      </c>
-      <c r="M88" t="s">
-        <v>645</v>
-      </c>
-      <c r="N88" t="s">
-        <v>23</v>
-      </c>
-      <c r="O88" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>647</v>
-      </c>
-      <c r="B89" t="s">
-        <v>138</v>
-      </c>
-      <c r="C89" t="s">
-        <v>17</v>
-      </c>
-      <c r="D89" t="s">
-        <v>27</v>
-      </c>
-      <c r="E89" t="s">
-        <v>648</v>
-      </c>
-      <c r="F89" t="s">
-        <v>649</v>
-      </c>
-      <c r="G89" t="s">
-        <v>94</v>
-      </c>
-      <c r="H89" t="s">
-        <v>650</v>
-      </c>
-      <c r="I89" t="s">
-        <v>17</v>
-      </c>
-      <c r="J89" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>652</v>
-      </c>
-      <c r="B90" t="s">
-        <v>466</v>
-      </c>
-      <c r="C90" t="s">
-        <v>17</v>
-      </c>
-      <c r="D90" t="s">
-        <v>63</v>
-      </c>
-      <c r="E90" t="s">
-        <v>653</v>
-      </c>
-      <c r="F90" t="s">
-        <v>654</v>
-      </c>
-      <c r="G90" t="s">
-        <v>104</v>
-      </c>
-      <c r="H90" t="s">
-        <v>655</v>
-      </c>
-      <c r="I90" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" t="s">
-        <v>656</v>
-      </c>
-      <c r="K90" t="s">
-        <v>657</v>
-      </c>
-      <c r="L90" t="s">
-        <v>76</v>
-      </c>
-      <c r="M90" t="s">
-        <v>658</v>
-      </c>
-      <c r="N90" t="s">
-        <v>23</v>
-      </c>
-      <c r="O90" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>660</v>
-      </c>
-      <c r="B91" t="s">
-        <v>90</v>
-      </c>
-      <c r="C91" t="s">
-        <v>17</v>
-      </c>
-      <c r="D91" t="s">
-        <v>311</v>
-      </c>
-      <c r="E91" t="s">
-        <v>661</v>
-      </c>
-      <c r="F91" t="s">
-        <v>662</v>
-      </c>
-      <c r="G91" t="s">
-        <v>94</v>
-      </c>
-      <c r="H91" t="s">
-        <v>663</v>
-      </c>
-      <c r="I91" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>665</v>
-      </c>
-      <c r="B92" t="s">
-        <v>666</v>
-      </c>
-      <c r="C92" t="s">
-        <v>23</v>
-      </c>
-      <c r="D92" t="s">
-        <v>63</v>
-      </c>
-      <c r="E92" t="s">
-        <v>667</v>
-      </c>
-      <c r="F92" t="s">
-        <v>167</v>
-      </c>
-      <c r="G92" t="s">
-        <v>37</v>
-      </c>
-      <c r="H92" t="s">
-        <v>668</v>
-      </c>
-      <c r="I92" t="s">
-        <v>17</v>
-      </c>
-      <c r="J92" t="s">
-        <v>669</v>
-      </c>
-      <c r="K92" t="s">
-        <v>670</v>
-      </c>
-      <c r="L92" t="s">
-        <v>94</v>
-      </c>
-      <c r="M92" t="s">
-        <v>671</v>
-      </c>
-      <c r="N92" t="s">
-        <v>23</v>
-      </c>
-      <c r="O92" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>673</v>
-      </c>
-      <c r="B93" t="s">
-        <v>320</v>
-      </c>
-      <c r="C93" t="s">
-        <v>23</v>
-      </c>
-      <c r="D93" t="s">
-        <v>63</v>
-      </c>
-      <c r="E93" t="s">
-        <v>674</v>
-      </c>
-      <c r="F93" t="s">
-        <v>675</v>
-      </c>
-      <c r="G93" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" t="s">
-        <v>676</v>
-      </c>
-      <c r="I93" t="s">
-        <v>17</v>
-      </c>
-      <c r="J93" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>510</v>
-      </c>
-      <c r="B94" t="s">
-        <v>678</v>
-      </c>
-      <c r="C94" t="s">
-        <v>23</v>
-      </c>
-      <c r="D94" t="s">
-        <v>268</v>
-      </c>
-      <c r="E94" t="s">
-        <v>679</v>
-      </c>
-      <c r="F94" t="s">
-        <v>680</v>
-      </c>
-      <c r="G94" t="s">
-        <v>94</v>
-      </c>
-      <c r="H94" t="s">
-        <v>681</v>
-      </c>
-      <c r="I94" t="s">
-        <v>17</v>
-      </c>
-      <c r="J94" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>683</v>
-      </c>
-      <c r="B95" t="s">
-        <v>684</v>
-      </c>
-      <c r="C95" t="s">
-        <v>17</v>
-      </c>
-      <c r="D95" t="s">
-        <v>56</v>
-      </c>
-      <c r="E95" t="s">
-        <v>685</v>
-      </c>
-      <c r="F95" t="s">
-        <v>686</v>
-      </c>
-      <c r="G95" t="s">
-        <v>37</v>
-      </c>
-      <c r="H95" t="s">
-        <v>687</v>
-      </c>
-      <c r="I95" t="s">
-        <v>17</v>
-      </c>
-      <c r="J95" t="s">
-        <v>688</v>
-      </c>
-      <c r="K95" t="s">
-        <v>689</v>
-      </c>
-      <c r="L95" t="s">
-        <v>94</v>
-      </c>
-      <c r="M95" t="s">
-        <v>690</v>
-      </c>
-      <c r="N95" t="s">
-        <v>23</v>
-      </c>
-      <c r="O95" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>692</v>
-      </c>
-      <c r="B96" t="s">
-        <v>693</v>
-      </c>
-      <c r="C96" t="s">
-        <v>23</v>
-      </c>
-      <c r="D96" t="s">
-        <v>56</v>
-      </c>
-      <c r="E96" t="s">
-        <v>694</v>
-      </c>
-      <c r="F96" t="s">
-        <v>695</v>
-      </c>
-      <c r="G96" t="s">
-        <v>104</v>
-      </c>
-      <c r="H96" t="s">
-        <v>696</v>
-      </c>
-      <c r="I96" t="s">
-        <v>17</v>
-      </c>
-      <c r="J96" t="s">
-        <v>697</v>
-      </c>
-      <c r="K96" t="s">
-        <v>698</v>
-      </c>
-      <c r="L96" t="s">
-        <v>30</v>
-      </c>
-      <c r="M96" t="s">
-        <v>699</v>
-      </c>
-      <c r="N96" t="s">
-        <v>23</v>
-      </c>
-      <c r="O96" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>701</v>
-      </c>
-      <c r="B97" t="s">
-        <v>702</v>
-      </c>
-      <c r="C97" t="s">
-        <v>23</v>
-      </c>
-      <c r="D97" t="s">
-        <v>268</v>
-      </c>
-      <c r="E97" t="s">
-        <v>703</v>
-      </c>
-      <c r="F97" t="s">
-        <v>704</v>
-      </c>
-      <c r="G97" t="s">
-        <v>76</v>
-      </c>
-      <c r="H97" t="s">
-        <v>705</v>
-      </c>
-      <c r="I97" t="s">
-        <v>17</v>
-      </c>
-      <c r="J97" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>707</v>
-      </c>
-      <c r="B98" t="s">
-        <v>708</v>
-      </c>
-      <c r="C98" t="s">
-        <v>23</v>
-      </c>
-      <c r="D98" t="s">
-        <v>18</v>
-      </c>
-      <c r="E98" t="s">
-        <v>709</v>
-      </c>
-      <c r="F98" t="s">
-        <v>710</v>
-      </c>
-      <c r="G98" t="s">
-        <v>37</v>
-      </c>
-      <c r="H98" t="s">
-        <v>711</v>
-      </c>
-      <c r="I98" t="s">
-        <v>23</v>
-      </c>
-      <c r="J98" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>713</v>
-      </c>
-      <c r="B99" t="s">
-        <v>714</v>
-      </c>
-      <c r="C99" t="s">
-        <v>23</v>
-      </c>
-      <c r="D99" t="s">
-        <v>27</v>
-      </c>
-      <c r="E99" t="s">
-        <v>715</v>
-      </c>
-      <c r="F99" t="s">
-        <v>716</v>
-      </c>
-      <c r="G99" t="s">
-        <v>83</v>
-      </c>
-      <c r="H99" t="s">
-        <v>717</v>
-      </c>
-      <c r="I99" t="s">
-        <v>23</v>
-      </c>
-      <c r="J99" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>719</v>
-      </c>
-      <c r="B100" t="s">
-        <v>720</v>
-      </c>
-      <c r="C100" t="s">
-        <v>17</v>
-      </c>
-      <c r="D100" t="s">
-        <v>27</v>
-      </c>
-      <c r="E100" t="s">
-        <v>721</v>
-      </c>
-      <c r="F100" t="s">
-        <v>722</v>
-      </c>
-      <c r="G100" t="s">
-        <v>94</v>
-      </c>
-      <c r="H100" t="s">
-        <v>723</v>
-      </c>
-      <c r="I100" t="s">
-        <v>17</v>
-      </c>
-      <c r="J100" t="s">
-        <v>724</v>
-      </c>
-      <c r="K100" t="s">
-        <v>725</v>
-      </c>
-      <c r="L100" t="s">
-        <v>94</v>
-      </c>
-      <c r="M100" t="s">
-        <v>726</v>
-      </c>
-      <c r="N100" t="s">
-        <v>23</v>
-      </c>
-      <c r="O100" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>728</v>
-      </c>
-      <c r="B101" t="s">
-        <v>729</v>
-      </c>
-      <c r="C101" t="s">
-        <v>23</v>
-      </c>
-      <c r="D101" t="s">
-        <v>49</v>
-      </c>
-      <c r="E101" t="s">
-        <v>730</v>
-      </c>
-      <c r="F101" t="s">
-        <v>731</v>
-      </c>
-      <c r="G101" t="s">
-        <v>30</v>
-      </c>
-      <c r="H101" t="s">
-        <v>732</v>
-      </c>
-      <c r="I101" t="s">
-        <v>23</v>
-      </c>
-      <c r="J101" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>734</v>
-      </c>
-      <c r="B102" t="s">
-        <v>735</v>
-      </c>
-      <c r="C102" t="s">
-        <v>17</v>
-      </c>
-      <c r="D102" t="s">
-        <v>73</v>
-      </c>
-      <c r="E102" t="s">
-        <v>736</v>
-      </c>
-      <c r="F102" t="s">
-        <v>113</v>
-      </c>
-      <c r="G102" t="s">
-        <v>83</v>
-      </c>
-      <c r="H102" t="s">
-        <v>737</v>
-      </c>
-      <c r="I102" t="s">
-        <v>17</v>
-      </c>
-      <c r="J102" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>739</v>
-      </c>
-      <c r="B103" t="s">
-        <v>740</v>
-      </c>
-      <c r="C103" t="s">
-        <v>17</v>
-      </c>
-      <c r="D103" t="s">
-        <v>311</v>
-      </c>
-      <c r="E103" t="s">
-        <v>741</v>
-      </c>
-      <c r="F103" t="s">
-        <v>742</v>
-      </c>
-      <c r="G103" t="s">
-        <v>83</v>
-      </c>
-      <c r="H103" t="s">
-        <v>743</v>
-      </c>
-      <c r="I103" t="s">
-        <v>23</v>
-      </c>
-      <c r="J103" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>602</v>
-      </c>
-      <c r="B104" t="s">
-        <v>745</v>
-      </c>
-      <c r="C104" t="s">
-        <v>17</v>
-      </c>
-      <c r="D104" t="s">
-        <v>49</v>
-      </c>
-      <c r="E104" t="s">
-        <v>746</v>
-      </c>
-      <c r="F104" t="s">
-        <v>747</v>
-      </c>
-      <c r="G104" t="s">
-        <v>37</v>
-      </c>
-      <c r="H104" t="s">
-        <v>748</v>
-      </c>
-      <c r="I104" t="s">
-        <v>17</v>
-      </c>
-      <c r="J104" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>750</v>
-      </c>
-      <c r="B105" t="s">
-        <v>751</v>
-      </c>
-      <c r="C105" t="s">
-        <v>23</v>
-      </c>
-      <c r="D105" t="s">
-        <v>311</v>
-      </c>
-      <c r="E105" t="s">
-        <v>752</v>
-      </c>
-      <c r="F105" t="s">
-        <v>753</v>
-      </c>
-      <c r="G105" t="s">
-        <v>30</v>
-      </c>
-      <c r="H105" t="s">
-        <v>754</v>
-      </c>
-      <c r="I105" t="s">
-        <v>17</v>
-      </c>
-      <c r="J105" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>756</v>
-      </c>
-      <c r="B106" t="s">
-        <v>757</v>
-      </c>
-      <c r="C106" t="s">
-        <v>23</v>
-      </c>
-      <c r="D106" t="s">
-        <v>91</v>
-      </c>
-      <c r="E106" t="s">
-        <v>758</v>
-      </c>
-      <c r="F106" t="s">
-        <v>759</v>
-      </c>
-      <c r="G106" t="s">
-        <v>94</v>
-      </c>
-      <c r="H106" t="s">
-        <v>760</v>
-      </c>
-      <c r="I106" t="s">
-        <v>23</v>
-      </c>
-      <c r="J106" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>762</v>
-      </c>
-      <c r="B107" t="s">
-        <v>763</v>
-      </c>
-      <c r="C107" t="s">
-        <v>17</v>
-      </c>
-      <c r="D107" t="s">
-        <v>18</v>
-      </c>
-      <c r="E107" t="s">
-        <v>764</v>
-      </c>
-      <c r="F107" t="s">
-        <v>765</v>
-      </c>
-      <c r="G107" t="s">
-        <v>37</v>
-      </c>
-      <c r="H107" t="s">
-        <v>766</v>
-      </c>
-      <c r="I107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J107" t="s">
-        <v>767</v>
-      </c>
-      <c r="K107" t="s">
-        <v>768</v>
-      </c>
-      <c r="L107" t="s">
-        <v>104</v>
-      </c>
-      <c r="M107" t="s">
-        <v>769</v>
-      </c>
-      <c r="N107" t="s">
-        <v>23</v>
-      </c>
-      <c r="O107" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>771</v>
-      </c>
-      <c r="B108" t="s">
-        <v>772</v>
-      </c>
-      <c r="C108" t="s">
-        <v>17</v>
-      </c>
-      <c r="D108" t="s">
-        <v>56</v>
-      </c>
-      <c r="E108" t="s">
-        <v>773</v>
-      </c>
-      <c r="F108" t="s">
-        <v>774</v>
-      </c>
-      <c r="G108" t="s">
-        <v>21</v>
-      </c>
-      <c r="H108" t="s">
-        <v>775</v>
-      </c>
-      <c r="I108" t="s">
-        <v>17</v>
-      </c>
-      <c r="J108" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>777</v>
-      </c>
-      <c r="B109" t="s">
-        <v>778</v>
-      </c>
-      <c r="C109" t="s">
-        <v>23</v>
-      </c>
-      <c r="D109" t="s">
-        <v>18</v>
-      </c>
-      <c r="E109" t="s">
-        <v>779</v>
-      </c>
-      <c r="F109" t="s">
-        <v>780</v>
-      </c>
-      <c r="G109" t="s">
-        <v>37</v>
-      </c>
-      <c r="H109" t="s">
-        <v>781</v>
-      </c>
-      <c r="I109" t="s">
-        <v>23</v>
-      </c>
-      <c r="J109" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>489</v>
-      </c>
-      <c r="B110" t="s">
-        <v>783</v>
-      </c>
-      <c r="C110" t="s">
-        <v>17</v>
-      </c>
-      <c r="D110" t="s">
-        <v>42</v>
-      </c>
-      <c r="E110" t="s">
-        <v>784</v>
-      </c>
-      <c r="F110" t="s">
-        <v>785</v>
-      </c>
-      <c r="G110" t="s">
-        <v>104</v>
-      </c>
-      <c r="H110" t="s">
-        <v>786</v>
-      </c>
-      <c r="I110" t="s">
-        <v>17</v>
-      </c>
-      <c r="J110" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>788</v>
-      </c>
-      <c r="B111" t="s">
-        <v>789</v>
-      </c>
-      <c r="C111" t="s">
-        <v>23</v>
-      </c>
-      <c r="D111" t="s">
-        <v>268</v>
-      </c>
-      <c r="E111" t="s">
-        <v>790</v>
-      </c>
-      <c r="F111" t="s">
-        <v>791</v>
-      </c>
-      <c r="G111" t="s">
-        <v>21</v>
-      </c>
-      <c r="H111" t="s">
-        <v>792</v>
-      </c>
-      <c r="I111" t="s">
-        <v>17</v>
-      </c>
-      <c r="J111" t="s">
-        <v>793</v>
-      </c>
-      <c r="K111" t="s">
-        <v>794</v>
-      </c>
-      <c r="L111" t="s">
-        <v>21</v>
-      </c>
-      <c r="M111" t="s">
-        <v>795</v>
-      </c>
-      <c r="N111" t="s">
-        <v>23</v>
-      </c>
-      <c r="O111" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>416</v>
-      </c>
-      <c r="B112" t="s">
-        <v>797</v>
-      </c>
-      <c r="C112" t="s">
-        <v>23</v>
-      </c>
-      <c r="D112" t="s">
-        <v>91</v>
-      </c>
-      <c r="E112" t="s">
-        <v>798</v>
-      </c>
-      <c r="F112" t="s">
-        <v>799</v>
-      </c>
-      <c r="G112" t="s">
-        <v>37</v>
-      </c>
-      <c r="H112" t="s">
-        <v>800</v>
-      </c>
-      <c r="I112" t="s">
-        <v>17</v>
-      </c>
-      <c r="J112" t="s">
-        <v>801</v>
-      </c>
-      <c r="K112" t="s">
-        <v>456</v>
-      </c>
-      <c r="L112" t="s">
-        <v>21</v>
-      </c>
-      <c r="M112" t="s">
-        <v>802</v>
-      </c>
-      <c r="N112" t="s">
-        <v>23</v>
-      </c>
-      <c r="O112" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>804</v>
-      </c>
-      <c r="B113" t="s">
-        <v>805</v>
-      </c>
-      <c r="C113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D113" t="s">
-        <v>311</v>
-      </c>
-      <c r="E113" t="s">
-        <v>806</v>
-      </c>
-      <c r="F113" t="s">
-        <v>807</v>
-      </c>
-      <c r="G113" t="s">
-        <v>94</v>
-      </c>
-      <c r="H113" t="s">
-        <v>808</v>
-      </c>
-      <c r="I113" t="s">
-        <v>17</v>
-      </c>
-      <c r="J113" t="s">
-        <v>809</v>
-      </c>
-      <c r="K113" t="s">
-        <v>810</v>
-      </c>
-      <c r="L113" t="s">
-        <v>104</v>
-      </c>
-      <c r="M113" t="s">
-        <v>811</v>
-      </c>
-      <c r="N113" t="s">
-        <v>23</v>
-      </c>
-      <c r="O113" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>813</v>
-      </c>
-      <c r="B114" t="s">
-        <v>814</v>
-      </c>
-      <c r="C114" t="s">
-        <v>17</v>
-      </c>
-      <c r="D114" t="s">
-        <v>18</v>
-      </c>
-      <c r="E114" t="s">
-        <v>815</v>
-      </c>
-      <c r="F114" t="s">
-        <v>816</v>
-      </c>
-      <c r="G114" t="s">
-        <v>37</v>
-      </c>
-      <c r="H114" t="s">
-        <v>817</v>
-      </c>
-      <c r="I114" t="s">
-        <v>17</v>
-      </c>
-      <c r="J114" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>819</v>
-      </c>
-      <c r="B115" t="s">
-        <v>820</v>
-      </c>
-      <c r="C115" t="s">
-        <v>23</v>
-      </c>
-      <c r="D115" t="s">
-        <v>27</v>
-      </c>
-      <c r="E115" t="s">
-        <v>821</v>
-      </c>
-      <c r="F115" t="s">
-        <v>822</v>
-      </c>
-      <c r="G115" t="s">
-        <v>94</v>
-      </c>
-      <c r="H115" t="s">
-        <v>823</v>
-      </c>
-      <c r="I115" t="s">
-        <v>17</v>
-      </c>
-      <c r="J115" t="s">
-        <v>824</v>
-      </c>
-      <c r="K115" t="s">
-        <v>825</v>
-      </c>
-      <c r="L115" t="s">
-        <v>21</v>
-      </c>
-      <c r="M115" t="s">
-        <v>826</v>
-      </c>
-      <c r="N115" t="s">
-        <v>23</v>
-      </c>
-      <c r="O115" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>828</v>
-      </c>
-      <c r="B116" t="s">
-        <v>829</v>
-      </c>
-      <c r="C116" t="s">
-        <v>17</v>
-      </c>
-      <c r="D116" t="s">
-        <v>63</v>
-      </c>
-      <c r="E116" t="s">
-        <v>830</v>
-      </c>
-      <c r="F116" t="s">
-        <v>831</v>
-      </c>
-      <c r="G116" t="s">
-        <v>104</v>
-      </c>
-      <c r="H116" t="s">
-        <v>832</v>
-      </c>
-      <c r="I116" t="s">
-        <v>17</v>
-      </c>
-      <c r="J116" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>834</v>
-      </c>
-      <c r="B117" t="s">
-        <v>835</v>
-      </c>
-      <c r="C117" t="s">
-        <v>23</v>
-      </c>
-      <c r="D117" t="s">
-        <v>91</v>
-      </c>
-      <c r="E117" t="s">
-        <v>836</v>
-      </c>
-      <c r="F117" t="s">
-        <v>837</v>
-      </c>
-      <c r="G117" t="s">
-        <v>21</v>
-      </c>
-      <c r="H117" t="s">
-        <v>838</v>
-      </c>
-      <c r="I117" t="s">
-        <v>17</v>
-      </c>
-      <c r="J117" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>840</v>
-      </c>
-      <c r="B118" t="s">
-        <v>841</v>
-      </c>
-      <c r="C118" t="s">
-        <v>23</v>
-      </c>
-      <c r="D118" t="s">
-        <v>18</v>
-      </c>
-      <c r="E118" t="s">
-        <v>842</v>
-      </c>
-      <c r="F118" t="s">
-        <v>448</v>
-      </c>
-      <c r="G118" t="s">
-        <v>94</v>
-      </c>
-      <c r="H118" t="s">
-        <v>843</v>
-      </c>
-      <c r="I118" t="s">
-        <v>17</v>
-      </c>
-      <c r="J118" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>845</v>
-      </c>
-      <c r="B119" t="s">
-        <v>80</v>
-      </c>
-      <c r="C119" t="s">
-        <v>17</v>
-      </c>
-      <c r="D119" t="s">
-        <v>42</v>
-      </c>
-      <c r="E119" t="s">
-        <v>846</v>
-      </c>
-      <c r="F119" t="s">
-        <v>847</v>
-      </c>
-      <c r="G119" t="s">
-        <v>83</v>
-      </c>
-      <c r="H119" t="s">
-        <v>848</v>
-      </c>
-      <c r="I119" t="s">
-        <v>17</v>
-      </c>
-      <c r="J119" t="s">
-        <v>849</v>
-      </c>
-      <c r="K119" t="s">
-        <v>552</v>
-      </c>
-      <c r="L119" t="s">
-        <v>94</v>
-      </c>
-      <c r="M119" t="s">
-        <v>850</v>
-      </c>
-      <c r="N119" t="s">
-        <v>23</v>
-      </c>
-      <c r="O119" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>852</v>
-      </c>
-      <c r="B120" t="s">
-        <v>394</v>
-      </c>
-      <c r="C120" t="s">
-        <v>23</v>
-      </c>
-      <c r="D120" t="s">
-        <v>18</v>
-      </c>
-      <c r="E120" t="s">
-        <v>853</v>
-      </c>
-      <c r="F120" t="s">
-        <v>854</v>
-      </c>
-      <c r="G120" t="s">
-        <v>83</v>
-      </c>
-      <c r="H120" t="s">
-        <v>855</v>
-      </c>
-      <c r="I120" t="s">
-        <v>17</v>
-      </c>
-      <c r="J120" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>857</v>
-      </c>
-      <c r="B121" t="s">
-        <v>639</v>
-      </c>
-      <c r="C121" t="s">
-        <v>23</v>
-      </c>
-      <c r="D121" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" t="s">
-        <v>858</v>
-      </c>
-      <c r="F121" t="s">
-        <v>794</v>
-      </c>
-      <c r="G121" t="s">
-        <v>30</v>
-      </c>
-      <c r="H121" t="s">
-        <v>859</v>
-      </c>
-      <c r="I121" t="s">
-        <v>23</v>
-      </c>
-      <c r="J121" t="s">
-        <v>860</v>
       </c>
     </row>
   </sheetData>
@@ -7962,21 +5692,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>861</v>
+        <v>601</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>862</v>
+        <v>602</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>863</v>
+        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>864</v>
+        <v>604</v>
       </c>
       <c r="B2" t="s">
-        <v>865</v>
+        <v>605</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -7985,24 +5715,24 @@
         <v>311</v>
       </c>
       <c r="E2" t="s">
-        <v>866</v>
+        <v>606</v>
       </c>
       <c r="F2" t="s">
-        <v>867</v>
+        <v>607</v>
       </c>
       <c r="G2" t="s">
-        <v>868</v>
+        <v>608</v>
       </c>
       <c r="H2" t="s">
-        <v>869</v>
+        <v>609</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>870</v>
+        <v>610</v>
       </c>
       <c r="B3" t="s">
-        <v>871</v>
+        <v>611</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -8011,24 +5741,24 @@
         <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>872</v>
+        <v>612</v>
       </c>
       <c r="F3" t="s">
-        <v>873</v>
+        <v>613</v>
       </c>
       <c r="G3" t="s">
-        <v>874</v>
+        <v>614</v>
       </c>
       <c r="H3" t="s">
-        <v>875</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>876</v>
+        <v>616</v>
       </c>
       <c r="B4" t="s">
-        <v>877</v>
+        <v>617</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -8037,24 +5767,24 @@
         <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>878</v>
+        <v>618</v>
       </c>
       <c r="F4" t="s">
-        <v>879</v>
+        <v>619</v>
       </c>
       <c r="G4" t="s">
-        <v>880</v>
+        <v>620</v>
       </c>
       <c r="H4" t="s">
-        <v>881</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>882</v>
+        <v>622</v>
       </c>
       <c r="B5" t="s">
-        <v>883</v>
+        <v>623</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -8063,24 +5793,24 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>884</v>
+        <v>624</v>
       </c>
       <c r="F5" t="s">
-        <v>885</v>
+        <v>625</v>
       </c>
       <c r="G5" t="s">
-        <v>886</v>
+        <v>626</v>
       </c>
       <c r="H5" t="s">
-        <v>887</v>
+        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>888</v>
+        <v>628</v>
       </c>
       <c r="B6" t="s">
-        <v>889</v>
+        <v>629</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -8089,24 +5819,24 @@
         <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>890</v>
+        <v>630</v>
       </c>
       <c r="F6" t="s">
-        <v>891</v>
+        <v>631</v>
       </c>
       <c r="G6" t="s">
-        <v>892</v>
+        <v>632</v>
       </c>
       <c r="H6" t="s">
-        <v>893</v>
+        <v>633</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>894</v>
+        <v>634</v>
       </c>
       <c r="B7" t="s">
-        <v>895</v>
+        <v>635</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -8115,24 +5845,24 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>896</v>
+        <v>636</v>
       </c>
       <c r="F7" t="s">
-        <v>897</v>
+        <v>637</v>
       </c>
       <c r="G7" t="s">
-        <v>898</v>
+        <v>638</v>
       </c>
       <c r="H7" t="s">
-        <v>899</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>900</v>
+        <v>640</v>
       </c>
       <c r="B8" t="s">
-        <v>901</v>
+        <v>641</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -8141,16 +5871,16 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>902</v>
+        <v>642</v>
       </c>
       <c r="F8" t="s">
-        <v>903</v>
+        <v>643</v>
       </c>
       <c r="G8" t="s">
-        <v>904</v>
+        <v>644</v>
       </c>
       <c r="H8" t="s">
-        <v>905</v>
+        <v>645</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -8158,7 +5888,7 @@
         <v>538</v>
       </c>
       <c r="B9" t="s">
-        <v>906</v>
+        <v>646</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -8167,24 +5897,24 @@
         <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>907</v>
+        <v>647</v>
       </c>
       <c r="F9" t="s">
-        <v>908</v>
+        <v>648</v>
       </c>
       <c r="G9" t="s">
-        <v>909</v>
+        <v>649</v>
       </c>
       <c r="H9" t="s">
-        <v>910</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>911</v>
+        <v>651</v>
       </c>
       <c r="B10" t="s">
-        <v>912</v>
+        <v>652</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -8193,24 +5923,24 @@
         <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>913</v>
+        <v>653</v>
       </c>
       <c r="F10" t="s">
-        <v>914</v>
+        <v>654</v>
       </c>
       <c r="G10" t="s">
-        <v>892</v>
+        <v>632</v>
       </c>
       <c r="H10" t="s">
-        <v>915</v>
+        <v>655</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>777</v>
+        <v>600</v>
       </c>
       <c r="B11" t="s">
-        <v>916</v>
+        <v>656</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -8219,24 +5949,24 @@
         <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>917</v>
+        <v>657</v>
       </c>
       <c r="F11" t="s">
-        <v>918</v>
+        <v>658</v>
       </c>
       <c r="G11" t="s">
-        <v>919</v>
+        <v>659</v>
       </c>
       <c r="H11" t="s">
-        <v>920</v>
+        <v>660</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>921</v>
+        <v>661</v>
       </c>
       <c r="B12" t="s">
-        <v>922</v>
+        <v>662</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -8245,24 +5975,24 @@
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>923</v>
+        <v>663</v>
       </c>
       <c r="F12" t="s">
-        <v>924</v>
+        <v>664</v>
       </c>
       <c r="G12" t="s">
-        <v>904</v>
+        <v>644</v>
       </c>
       <c r="H12" t="s">
-        <v>925</v>
+        <v>665</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>926</v>
+        <v>666</v>
       </c>
       <c r="B13" t="s">
-        <v>927</v>
+        <v>667</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -8271,24 +6001,24 @@
         <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>928</v>
+        <v>668</v>
       </c>
       <c r="F13" t="s">
-        <v>929</v>
+        <v>669</v>
       </c>
       <c r="G13" t="s">
-        <v>930</v>
+        <v>670</v>
       </c>
       <c r="H13" t="s">
-        <v>931</v>
+        <v>671</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>713</v>
+        <v>599</v>
       </c>
       <c r="B14" t="s">
-        <v>932</v>
+        <v>672</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -8297,24 +6027,24 @@
         <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>933</v>
+        <v>673</v>
       </c>
       <c r="F14" t="s">
-        <v>934</v>
+        <v>674</v>
       </c>
       <c r="G14" t="s">
-        <v>935</v>
+        <v>675</v>
       </c>
       <c r="H14" t="s">
-        <v>936</v>
+        <v>676</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>937</v>
+        <v>677</v>
       </c>
       <c r="B15" t="s">
-        <v>938</v>
+        <v>678</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -8323,24 +6053,24 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>939</v>
+        <v>679</v>
       </c>
       <c r="F15" t="s">
-        <v>940</v>
+        <v>680</v>
       </c>
       <c r="G15" t="s">
-        <v>941</v>
+        <v>681</v>
       </c>
       <c r="H15" t="s">
-        <v>942</v>
+        <v>682</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>943</v>
+        <v>683</v>
       </c>
       <c r="B16" t="s">
-        <v>944</v>
+        <v>684</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -8349,24 +6079,24 @@
         <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>945</v>
+        <v>685</v>
       </c>
       <c r="F16" t="s">
-        <v>946</v>
+        <v>686</v>
       </c>
       <c r="G16" t="s">
-        <v>947</v>
+        <v>687</v>
       </c>
       <c r="H16" t="s">
-        <v>948</v>
+        <v>688</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>949</v>
+        <v>689</v>
       </c>
       <c r="B17" t="s">
-        <v>950</v>
+        <v>690</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -8375,24 +6105,24 @@
         <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>951</v>
+        <v>691</v>
       </c>
       <c r="F17" t="s">
-        <v>952</v>
+        <v>692</v>
       </c>
       <c r="G17" t="s">
-        <v>904</v>
+        <v>644</v>
       </c>
       <c r="H17" t="s">
-        <v>953</v>
+        <v>693</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>954</v>
+        <v>694</v>
       </c>
       <c r="B18" t="s">
-        <v>955</v>
+        <v>695</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -8401,24 +6131,24 @@
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>956</v>
+        <v>696</v>
       </c>
       <c r="F18" t="s">
-        <v>957</v>
+        <v>697</v>
       </c>
       <c r="G18" t="s">
-        <v>958</v>
+        <v>698</v>
       </c>
       <c r="H18" t="s">
-        <v>893</v>
+        <v>633</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>959</v>
+        <v>699</v>
       </c>
       <c r="B19" t="s">
-        <v>960</v>
+        <v>700</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -8427,16 +6157,16 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>961</v>
+        <v>701</v>
       </c>
       <c r="F19" t="s">
-        <v>962</v>
+        <v>702</v>
       </c>
       <c r="G19" t="s">
-        <v>963</v>
+        <v>703</v>
       </c>
       <c r="H19" t="s">
-        <v>964</v>
+        <v>704</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -8444,7 +6174,7 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>965</v>
+        <v>705</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -8453,24 +6183,24 @@
         <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>966</v>
+        <v>706</v>
       </c>
       <c r="F20" t="s">
-        <v>967</v>
+        <v>707</v>
       </c>
       <c r="G20" t="s">
-        <v>968</v>
+        <v>708</v>
       </c>
       <c r="H20" t="s">
-        <v>969</v>
+        <v>709</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>970</v>
+        <v>710</v>
       </c>
       <c r="B21" t="s">
-        <v>971</v>
+        <v>711</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -8479,16 +6209,16 @@
         <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>972</v>
+        <v>712</v>
       </c>
       <c r="F21" t="s">
-        <v>973</v>
+        <v>713</v>
       </c>
       <c r="G21" t="s">
-        <v>919</v>
+        <v>659</v>
       </c>
       <c r="H21" t="s">
-        <v>915</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>